<commit_message>
quarta vez da commitada
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -1,25 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\OneDrive\Desktop\ff\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDE83FA-44D4-4F4D-8BEA-C7A503626A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +347,958 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+      <c r="M1">
+        <v>1</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="O1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f>SUM(D1:D3)</f>
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>22221</v>
+      </c>
+      <c r="G8">
+        <v>22221</v>
+      </c>
+      <c r="H8">
+        <v>22221</v>
+      </c>
+      <c r="I8">
+        <v>22221</v>
+      </c>
+      <c r="J8">
+        <v>22221</v>
+      </c>
+      <c r="K8">
+        <v>22221</v>
+      </c>
+      <c r="L8">
+        <v>22221</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>